<commit_message>
refact: level 관련 테이블 수정 (LeveStageTable)
</commit_message>
<xml_diff>
--- a/Document/GameTable/Level/LevelStageTable.xlsx
+++ b/Document/GameTable/Level/LevelStageTable.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HJ\Documents\Unreal Projects\ProjectBS\Document\GameTable\Level\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05ED555-4E49-46CB-9FBC-2B6B8428F5EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD06590-4962-42BB-9D8B-F5AE250ABE24}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
   <si>
     <t>Name</t>
   </si>
@@ -70,9 +70,6 @@
     <t>stage1</t>
   </si>
   <si>
-    <t>"Basic_level11"</t>
-  </si>
-  <si>
     <t>(8,8)</t>
   </si>
   <si>
@@ -83,6 +80,18 @@
   </si>
   <si>
     <t>"늪지대"</t>
+  </si>
+  <si>
+    <t>Basic_level11</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Basic_level12</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>stage2</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -1034,10 +1043,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1102,25 +1111,25 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="D2">
         <v>1000</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G2">
         <v>10</v>
       </c>
       <c r="H2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" t="s">
         <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
       </c>
       <c r="J2" t="b">
         <v>0</v>
@@ -1129,7 +1138,7 @@
         <v>1</v>
       </c>
       <c r="L2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M2">
         <v>100</v>
@@ -1138,11 +1147,59 @@
         <v>0.2</v>
       </c>
       <c r="O2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
+      <c r="H3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" t="s">
+        <v>18</v>
+      </c>
+      <c r="J3" t="b">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>1</v>
+      </c>
+      <c r="L3" t="s">
+        <v>19</v>
+      </c>
+      <c r="M3">
+        <v>100</v>
+      </c>
+      <c r="N3">
+        <v>0.2</v>
+      </c>
+      <c r="O3">
         <v>0.3</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>